<commit_message>
Adicionado classes de inimigos
</commit_message>
<xml_diff>
--- a/assets/dados.xlsx
+++ b/assets/dados.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\Treinamentos\Python\meu-jogo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\Treinamentos\Python\meu-jogo\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF22EDCD-53A8-4981-9933-F670B97B3726}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17EFC72B-C577-41BD-83C1-2464CBC4E2F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{D0AC3F4F-C2BF-45A5-B453-A20E0A07E23C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="85">
   <si>
     <t>LARGURA</t>
   </si>
@@ -261,6 +261,36 @@
   </si>
   <si>
     <t>6B</t>
+  </si>
+  <si>
+    <t>3C</t>
+  </si>
+  <si>
+    <t>7A</t>
+  </si>
+  <si>
+    <t>7B</t>
+  </si>
+  <si>
+    <t>8A</t>
+  </si>
+  <si>
+    <t>8B</t>
+  </si>
+  <si>
+    <t>8C</t>
+  </si>
+  <si>
+    <t>9A</t>
+  </si>
+  <si>
+    <t>9B</t>
+  </si>
+  <si>
+    <t>9C</t>
+  </si>
+  <si>
+    <t>9D</t>
   </si>
 </sst>
 </file>
@@ -312,7 +342,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -340,6 +370,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFEFF1FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA9D0FD"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -463,7 +505,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -568,6 +610,24 @@
     <xf numFmtId="2" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -592,14 +652,116 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="52">
+  <dxfs count="76">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFA9D0FD"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.00000"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -628,6 +790,25 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -654,6 +835,25 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -676,6 +876,25 @@
           <bgColor rgb="FFFFFAEB"/>
         </patternFill>
       </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -729,6 +948,198 @@
         <family val="3"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
       <numFmt numFmtId="1" formatCode="0"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -757,154 +1168,305 @@
         <family val="3"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="164" formatCode="0.00000"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFA9D0FD"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border outline="0">
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.00000"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.00000"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFAEB"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.00000"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFAEB"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.00000"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFAEB"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.00000"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFAEB"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
+        <right/>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
       <font>
         <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Consolas"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Consolas"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Consolas"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Consolas"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Consolas"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="0.00000"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Consolas"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Consolas"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -1067,7 +1629,13 @@
         <family val="3"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1087,6 +1655,34 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Consolas"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1734,6 +2330,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFA9D0FD"/>
       <color rgb="FFEFF1FF"/>
       <color rgb="FFF7F7F7"/>
       <color rgb="FFFFFAEB"/>
@@ -1751,21 +2348,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5CEE69C6-A5FC-48AE-B07B-580AA6919BDF}" name="Tabela2" displayName="Tabela2" ref="C2:D3" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5CEE69C6-A5FC-48AE-B07B-580AA6919BDF}" name="Tabela2" displayName="Tabela2" ref="C2:D3" totalsRowShown="0" headerRowDxfId="75" dataDxfId="74">
   <autoFilter ref="C2:D3" xr:uid="{5CEE69C6-A5FC-48AE-B07B-580AA6919BDF}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{19FE746F-44B9-4BB5-91D8-51A23F72B0F3}" name="LARGURA" dataDxfId="49"/>
-    <tableColumn id="2" xr3:uid="{CAA8343F-A076-4123-903E-D9710A238A7B}" name="ALTURA" dataDxfId="48"/>
+    <tableColumn id="1" xr3:uid="{19FE746F-44B9-4BB5-91D8-51A23F72B0F3}" name="LARGURA" dataDxfId="73"/>
+    <tableColumn id="2" xr3:uid="{CAA8343F-A076-4123-903E-D9710A238A7B}" name="ALTURA" dataDxfId="72"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8DC9FD6E-1F8C-47DE-9BDA-84956E9A7D1A}" name="Dados" displayName="Dados" ref="B5:J88" headerRowDxfId="47" dataDxfId="46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8DC9FD6E-1F8C-47DE-9BDA-84956E9A7D1A}" name="Dados" displayName="Dados" ref="B5:J88" headerRowDxfId="71" dataDxfId="70">
   <autoFilter ref="B5:J88" xr:uid="{8DC9FD6E-1F8C-47DE-9BDA-84956E9A7D1A}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -1778,21 +2375,21 @@
     <filterColumn colId="8" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="9">
-    <tableColumn id="9" xr3:uid="{0DF3B7F9-552C-4CC3-A117-90EA55623D53}" name="Hn" totalsRowLabel="Total" dataDxfId="45" totalsRowDxfId="44"/>
-    <tableColumn id="1" xr3:uid="{DE0DA5D4-D475-44A5-8F1B-07F110C8575D}" name="Xo" dataDxfId="43" totalsRowDxfId="42"/>
-    <tableColumn id="2" xr3:uid="{F93231F0-EEC3-47C6-95AF-D1F7526D2F12}" name="Yo" dataDxfId="41" totalsRowDxfId="40"/>
-    <tableColumn id="10" xr3:uid="{8151CCAC-10D2-4DBE-90A5-9FE4EB068CCF}" name="Lx" dataDxfId="39" totalsRowDxfId="38"/>
-    <tableColumn id="11" xr3:uid="{36A9D561-02F9-4894-B94E-5A479EA700F6}" name="Ly" dataDxfId="37" totalsRowDxfId="36"/>
-    <tableColumn id="3" xr3:uid="{551AEAA0-B086-4B03-BBB5-2803FD04E8F6}" name="%X" dataDxfId="35" totalsRowDxfId="34">
+    <tableColumn id="9" xr3:uid="{0DF3B7F9-552C-4CC3-A117-90EA55623D53}" name="Hn" totalsRowLabel="Total" dataDxfId="69" totalsRowDxfId="68"/>
+    <tableColumn id="1" xr3:uid="{DE0DA5D4-D475-44A5-8F1B-07F110C8575D}" name="Xo" dataDxfId="67" totalsRowDxfId="66"/>
+    <tableColumn id="2" xr3:uid="{F93231F0-EEC3-47C6-95AF-D1F7526D2F12}" name="Yo" dataDxfId="65" totalsRowDxfId="64"/>
+    <tableColumn id="10" xr3:uid="{8151CCAC-10D2-4DBE-90A5-9FE4EB068CCF}" name="Lx" dataDxfId="63" totalsRowDxfId="62"/>
+    <tableColumn id="11" xr3:uid="{36A9D561-02F9-4894-B94E-5A479EA700F6}" name="Ly" dataDxfId="61" totalsRowDxfId="60"/>
+    <tableColumn id="3" xr3:uid="{551AEAA0-B086-4B03-BBB5-2803FD04E8F6}" name="%X" dataDxfId="59" totalsRowDxfId="58">
       <calculatedColumnFormula>C6/$C$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{4006C018-F747-492B-B912-3309C080FF5B}" name="%Y" dataDxfId="33" totalsRowDxfId="32">
+    <tableColumn id="4" xr3:uid="{4006C018-F747-492B-B912-3309C080FF5B}" name="%Y" dataDxfId="57" totalsRowDxfId="56">
       <calculatedColumnFormula>D6/$D$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{96A9D100-76DF-4E87-8D7A-1787C8EF65AD}" name="%Lx" dataDxfId="31" totalsRowDxfId="30">
+    <tableColumn id="7" xr3:uid="{96A9D100-76DF-4E87-8D7A-1787C8EF65AD}" name="%Lx" dataDxfId="55" totalsRowDxfId="54">
       <calculatedColumnFormula>E6/$C$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{987E49E0-1602-42D6-8B47-858DCCD5F507}" name="%Ly" totalsRowFunction="sum" dataDxfId="29" totalsRowDxfId="28">
+    <tableColumn id="8" xr3:uid="{987E49E0-1602-42D6-8B47-858DCCD5F507}" name="%Ly" totalsRowFunction="sum" dataDxfId="53" totalsRowDxfId="52">
       <calculatedColumnFormula>F6/$D$3</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1801,22 +2398,22 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B9B91532-1A6D-4BFD-A3C9-FE5198A9D833}" name="Tabela3" displayName="Tabela3" ref="C2:D3" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B9B91532-1A6D-4BFD-A3C9-FE5198A9D833}" name="Tabela3" displayName="Tabela3" ref="C2:D3" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50">
   <autoFilter ref="C2:D3" xr:uid="{B9B91532-1A6D-4BFD-A3C9-FE5198A9D833}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{F5E6162D-FD52-46E2-8B43-60D07C7F0B05}" name="LARGURA" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{0536673C-422B-412E-B620-76259C87A4B1}" name="ALTURA" dataDxfId="24"/>
+    <tableColumn id="1" xr3:uid="{F5E6162D-FD52-46E2-8B43-60D07C7F0B05}" name="LARGURA" dataDxfId="49"/>
+    <tableColumn id="2" xr3:uid="{0536673C-422B-412E-B620-76259C87A4B1}" name="ALTURA" dataDxfId="48"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{939B5E52-38F6-48A4-AE26-2EC7130F684A}" name="Dados5" displayName="Dados5" ref="B5:J17" headerRowDxfId="23" dataDxfId="22">
-  <autoFilter ref="B5:J17" xr:uid="{939B5E52-38F6-48A4-AE26-2EC7130F684A}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{939B5E52-38F6-48A4-AE26-2EC7130F684A}" name="Dados5" displayName="Dados5" ref="B5:J20" headerRowDxfId="47" dataDxfId="46">
+  <autoFilter ref="B5:J20" xr:uid="{939B5E52-38F6-48A4-AE26-2EC7130F684A}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -1828,21 +2425,21 @@
     <filterColumn colId="8" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="9">
-    <tableColumn id="9" xr3:uid="{6E595570-22FB-4BE9-8B95-8853BB8C0B7A}" name="Qn" totalsRowLabel="Total" dataDxfId="4" totalsRowDxfId="21"/>
-    <tableColumn id="1" xr3:uid="{13A0E9E7-81D6-4A59-96AF-9DE2B186C82D}" name="Xo" dataDxfId="5" totalsRowDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{AB93CE08-B82A-4AA6-8240-2F5864B4A3E6}" name="Yo" dataDxfId="18" totalsRowDxfId="19"/>
-    <tableColumn id="10" xr3:uid="{FDFFD39A-91B4-4977-9F7B-13F1D8FF68B8}" name="Lx" dataDxfId="16" totalsRowDxfId="17"/>
-    <tableColumn id="11" xr3:uid="{7986F743-235C-4E83-9DDA-B0AA56FAAD57}" name="Ly" dataDxfId="14" totalsRowDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{642BB52F-5D8B-4526-B129-53CAF0F2CBC0}" name="%X" dataDxfId="3" totalsRowDxfId="13">
+    <tableColumn id="9" xr3:uid="{6E595570-22FB-4BE9-8B95-8853BB8C0B7A}" name="Qn" totalsRowLabel="Total" dataDxfId="45" totalsRowDxfId="44"/>
+    <tableColumn id="1" xr3:uid="{13A0E9E7-81D6-4A59-96AF-9DE2B186C82D}" name="Xo" dataDxfId="43" totalsRowDxfId="42"/>
+    <tableColumn id="2" xr3:uid="{AB93CE08-B82A-4AA6-8240-2F5864B4A3E6}" name="Yo" dataDxfId="41" totalsRowDxfId="40"/>
+    <tableColumn id="10" xr3:uid="{FDFFD39A-91B4-4977-9F7B-13F1D8FF68B8}" name="Lx" dataDxfId="39" totalsRowDxfId="38"/>
+    <tableColumn id="11" xr3:uid="{7986F743-235C-4E83-9DDA-B0AA56FAAD57}" name="Ly" dataDxfId="37" totalsRowDxfId="36"/>
+    <tableColumn id="3" xr3:uid="{642BB52F-5D8B-4526-B129-53CAF0F2CBC0}" name="%X" dataDxfId="35" totalsRowDxfId="34">
       <calculatedColumnFormula>C6/$C$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{79EA8C2C-0B71-4202-9967-FA51045C9BF8}" name="%Y" dataDxfId="2" totalsRowDxfId="12">
+    <tableColumn id="4" xr3:uid="{79EA8C2C-0B71-4202-9967-FA51045C9BF8}" name="%Y" dataDxfId="33" totalsRowDxfId="32">
       <calculatedColumnFormula>D6/$D$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{29BFC2C9-4E73-4677-9FD8-F836BE0F28CB}" name="%Lx" dataDxfId="1" totalsRowDxfId="11">
+    <tableColumn id="7" xr3:uid="{29BFC2C9-4E73-4677-9FD8-F836BE0F28CB}" name="%Lx" dataDxfId="31" totalsRowDxfId="30">
       <calculatedColumnFormula>E6/$C$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{E69446E8-B6B6-45C6-B132-85E121C49873}" name="%Ly" totalsRowFunction="sum" dataDxfId="0" totalsRowDxfId="10">
+    <tableColumn id="8" xr3:uid="{E69446E8-B6B6-45C6-B132-85E121C49873}" name="%Ly" totalsRowFunction="sum" dataDxfId="29" totalsRowDxfId="28">
       <calculatedColumnFormula>F6/$D$3</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1851,14 +2448,64 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{F4386F2F-A4B9-437F-AE23-A11AFAAFB546}" name="Tabela36" displayName="Tabela36" ref="C2:D3" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{F4386F2F-A4B9-437F-AE23-A11AFAAFB546}" name="Tabela36" displayName="Tabela36" ref="C2:D3" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
   <autoFilter ref="C2:D3" xr:uid="{F4386F2F-A4B9-437F-AE23-A11AFAAFB546}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{2BF3EB10-4E71-4448-A45B-20837FD1B36D}" name="LARGURA" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{D2EA38E6-5653-4058-9FA3-793B3CC44826}" name="ALTURA" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{2BF3EB10-4E71-4448-A45B-20837FD1B36D}" name="LARGURA" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{D2EA38E6-5653-4058-9FA3-793B3CC44826}" name="ALTURA" dataDxfId="24"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{12682A61-99E3-463D-B4BE-7160CA7EEFB6}" name="Dados57" displayName="Dados57" ref="B25:J43" headerRowDxfId="23" dataDxfId="22">
+  <autoFilter ref="B25:J43" xr:uid="{12682A61-99E3-463D-B4BE-7160CA7EEFB6}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+    <filterColumn colId="6" hiddenButton="1"/>
+    <filterColumn colId="7" hiddenButton="1"/>
+    <filterColumn colId="8" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="9">
+    <tableColumn id="9" xr3:uid="{BBF677B1-48B5-4DC7-9C97-7F47AED4B666}" name="Qn" totalsRowLabel="Total" dataDxfId="21" totalsRowDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{2677CE7B-8C2A-4D71-AD50-7D948C1965FA}" name="Xo" dataDxfId="19" totalsRowDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{A536A70C-052F-43A1-8B6A-8E1577AC352D}" name="Yo" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="10" xr3:uid="{4BEA4EA1-7D05-4ADC-B6EF-8F38551666CA}" name="Lx" dataDxfId="15" totalsRowDxfId="14"/>
+    <tableColumn id="11" xr3:uid="{F621153A-3657-41A6-87A1-1AF6A4FF6148}" name="Ly" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{029AE564-A09C-42DF-BC6B-D539CBEFB642}" name="%X" dataDxfId="11" totalsRowDxfId="10">
+      <calculatedColumnFormula>C26/$C$23</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{76D68A58-02F4-4F54-A880-D29ABB1EA7B1}" name="%Y" dataDxfId="9" totalsRowDxfId="8">
+      <calculatedColumnFormula>D26/$D$23</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{7E0ED985-B6D0-4C54-A1D7-49842BE05F0F}" name="%Lx" dataDxfId="7" totalsRowDxfId="6">
+      <calculatedColumnFormula>E26/$C$23</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{93B5276A-961A-47B2-AFCC-9E07FF625BF9}" name="%Ly" totalsRowFunction="sum" dataDxfId="5" totalsRowDxfId="4">
+      <calculatedColumnFormula>F26/$D$23</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{EF066055-C48F-4F66-ABA8-F3E19CCB97CC}" name="Tabela368" displayName="Tabela368" ref="C22:D23" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
+  <autoFilter ref="C22:D23" xr:uid="{EF066055-C48F-4F66-ABA8-F3E19CCB97CC}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{8D80C18B-9D2D-4323-B326-DD408277FAD1}" name="LARGURA" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{FD10CFD1-AA04-4ED5-85A5-B9771375992B}" name="ALTURA" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -2213,7 +2860,7 @@
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="42" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="7">
@@ -2232,7 +2879,7 @@
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="36"/>
+      <c r="B7" s="42"/>
       <c r="C7" s="7">
         <v>90</v>
       </c>
@@ -2249,7 +2896,7 @@
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="36"/>
+      <c r="B8" s="42"/>
       <c r="C8" s="7">
         <v>119</v>
       </c>
@@ -2266,7 +2913,7 @@
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="36"/>
+      <c r="B9" s="42"/>
       <c r="C9" s="7">
         <v>91</v>
       </c>
@@ -2283,7 +2930,7 @@
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="37"/>
+      <c r="B10" s="43"/>
       <c r="C10" s="8">
         <v>89</v>
       </c>
@@ -2300,7 +2947,7 @@
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="38" t="s">
+      <c r="B11" s="44" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="9">
@@ -2319,7 +2966,7 @@
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="39"/>
+      <c r="B12" s="45"/>
       <c r="C12" s="10">
         <v>166</v>
       </c>
@@ -2336,7 +2983,7 @@
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="39"/>
+      <c r="B13" s="45"/>
       <c r="C13" s="10">
         <v>106</v>
       </c>
@@ -2353,7 +3000,7 @@
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="40"/>
+      <c r="B14" s="46"/>
       <c r="C14" s="11">
         <v>74</v>
       </c>
@@ -2370,7 +3017,7 @@
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="41" t="s">
+      <c r="B15" s="47" t="s">
         <v>14</v>
       </c>
       <c r="C15" s="12">
@@ -2389,7 +3036,7 @@
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="42"/>
+      <c r="B16" s="48"/>
       <c r="C16" s="7">
         <v>38</v>
       </c>
@@ -2406,7 +3053,7 @@
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="42"/>
+      <c r="B17" s="48"/>
       <c r="C17" s="7">
         <v>20</v>
       </c>
@@ -2423,7 +3070,7 @@
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="43"/>
+      <c r="B18" s="49"/>
       <c r="C18" s="8">
         <v>18</v>
       </c>
@@ -2440,7 +3087,7 @@
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="38" t="s">
+      <c r="B19" s="44" t="s">
         <v>15</v>
       </c>
       <c r="C19" s="10">
@@ -2459,7 +3106,7 @@
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="39"/>
+      <c r="B20" s="45"/>
       <c r="C20" s="10">
         <v>180</v>
       </c>
@@ -2476,7 +3123,7 @@
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="39"/>
+      <c r="B21" s="45"/>
       <c r="C21" s="10">
         <v>162</v>
       </c>
@@ -2493,7 +3140,7 @@
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="40"/>
+      <c r="B22" s="46"/>
       <c r="C22" s="11">
         <v>160</v>
       </c>
@@ -5376,10 +6023,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1E46719-599A-4657-9139-C16D5FF7B306}">
-  <dimension ref="B1:J17"/>
+  <dimension ref="B1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5498,7 +6145,7 @@
         <v>0.1</v>
       </c>
       <c r="J6" s="23">
-        <f t="shared" ref="J6:J17" si="3">F6/$D$3</f>
+        <f t="shared" ref="J6:J18" si="3">F6/$D$3</f>
         <v>0.4</v>
       </c>
     </row>
@@ -5671,7 +6318,7 @@
       <c r="B12" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="C12" s="44">
+      <c r="C12" s="36">
         <v>8</v>
       </c>
       <c r="D12" s="14">
@@ -5704,7 +6351,7 @@
       <c r="B13" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="C13" s="44">
+      <c r="C13" s="36">
         <v>19</v>
       </c>
       <c r="D13" s="14">
@@ -5737,7 +6384,7 @@
       <c r="B14" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="C14" s="44">
+      <c r="C14" s="36">
         <v>5</v>
       </c>
       <c r="D14" s="14">
@@ -5770,7 +6417,7 @@
       <c r="B15" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="C15" s="44">
+      <c r="C15" s="36">
         <v>22</v>
       </c>
       <c r="D15" s="14">
@@ -5803,7 +6450,7 @@
       <c r="B16" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="C16" s="44">
+      <c r="C16" s="36">
         <v>8</v>
       </c>
       <c r="D16" s="14">
@@ -5836,7 +6483,7 @@
       <c r="B17" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="C17" s="44">
+      <c r="C17" s="36">
         <v>16</v>
       </c>
       <c r="D17" s="14">
@@ -5865,11 +6512,777 @@
         <v>0.1</v>
       </c>
     </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B18" s="30">
+        <v>7</v>
+      </c>
+      <c r="C18" s="36">
+        <v>8</v>
+      </c>
+      <c r="D18" s="14">
+        <v>10</v>
+      </c>
+      <c r="E18" s="13">
+        <v>14</v>
+      </c>
+      <c r="F18" s="13">
+        <v>6</v>
+      </c>
+      <c r="G18" s="22">
+        <f>C18/$C$3</f>
+        <v>0.26666666666666666</v>
+      </c>
+      <c r="H18" s="23">
+        <f>D18/$D$3</f>
+        <v>0.5</v>
+      </c>
+      <c r="I18" s="23">
+        <f>E18/$C$3</f>
+        <v>0.46666666666666667</v>
+      </c>
+      <c r="J18" s="23">
+        <f t="shared" si="3"/>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B19" s="30">
+        <v>8</v>
+      </c>
+      <c r="C19" s="36">
+        <v>11</v>
+      </c>
+      <c r="D19" s="14">
+        <v>7</v>
+      </c>
+      <c r="E19" s="13">
+        <v>8</v>
+      </c>
+      <c r="F19" s="13">
+        <v>3</v>
+      </c>
+      <c r="G19" s="22">
+        <f>C19/$C$3</f>
+        <v>0.36666666666666664</v>
+      </c>
+      <c r="H19" s="23">
+        <f>D19/$D$3</f>
+        <v>0.35</v>
+      </c>
+      <c r="I19" s="23">
+        <f>E19/$C$3</f>
+        <v>0.26666666666666666</v>
+      </c>
+      <c r="J19" s="23">
+        <f>F19/$D$3</f>
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B20" s="30">
+        <v>9</v>
+      </c>
+      <c r="C20" s="36">
+        <v>8</v>
+      </c>
+      <c r="D20" s="14">
+        <v>4</v>
+      </c>
+      <c r="E20" s="13">
+        <v>14</v>
+      </c>
+      <c r="F20" s="13">
+        <v>3</v>
+      </c>
+      <c r="G20" s="22">
+        <f>C20/$C$3</f>
+        <v>0.26666666666666666</v>
+      </c>
+      <c r="H20" s="23">
+        <f>D20/$D$3</f>
+        <v>0.2</v>
+      </c>
+      <c r="I20" s="23">
+        <f>E20/$C$3</f>
+        <v>0.46666666666666667</v>
+      </c>
+      <c r="J20" s="23">
+        <f>F20/$D$3</f>
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B22" s="2"/>
+      <c r="C22" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="D22" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B23" s="2"/>
+      <c r="C23" s="14">
+        <v>25</v>
+      </c>
+      <c r="D23" s="14">
+        <v>25</v>
+      </c>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B25" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="E25" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="F25" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="G25" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="H25" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="I25" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="J25" s="37" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B26" s="29">
+        <v>1</v>
+      </c>
+      <c r="C26" s="13">
+        <v>10</v>
+      </c>
+      <c r="D26" s="13">
+        <v>0</v>
+      </c>
+      <c r="E26" s="13">
+        <v>5</v>
+      </c>
+      <c r="F26" s="13">
+        <v>6</v>
+      </c>
+      <c r="G26" s="22">
+        <f t="shared" ref="G26:G43" si="4">C26/$C$23</f>
+        <v>0.4</v>
+      </c>
+      <c r="H26" s="23">
+        <f t="shared" ref="H26:H43" si="5">D26/$D$23</f>
+        <v>0</v>
+      </c>
+      <c r="I26" s="23">
+        <f t="shared" ref="I26:I43" si="6">E26/$C$23</f>
+        <v>0.2</v>
+      </c>
+      <c r="J26" s="23">
+        <f t="shared" ref="J26:J43" si="7">F26/$D$23</f>
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B27" s="30">
+        <v>2</v>
+      </c>
+      <c r="C27" s="36">
+        <v>3</v>
+      </c>
+      <c r="D27" s="14">
+        <v>6</v>
+      </c>
+      <c r="E27" s="13">
+        <v>19</v>
+      </c>
+      <c r="F27" s="13">
+        <v>4</v>
+      </c>
+      <c r="G27" s="22">
+        <f t="shared" si="4"/>
+        <v>0.12</v>
+      </c>
+      <c r="H27" s="23">
+        <f t="shared" si="5"/>
+        <v>0.24</v>
+      </c>
+      <c r="I27" s="23">
+        <f t="shared" si="6"/>
+        <v>0.76</v>
+      </c>
+      <c r="J27" s="23">
+        <f t="shared" si="7"/>
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B28" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="C28" s="36">
+        <v>1</v>
+      </c>
+      <c r="D28" s="14">
+        <v>10</v>
+      </c>
+      <c r="E28" s="13">
+        <v>6</v>
+      </c>
+      <c r="F28" s="13">
+        <v>2</v>
+      </c>
+      <c r="G28" s="22">
+        <f t="shared" si="4"/>
+        <v>0.04</v>
+      </c>
+      <c r="H28" s="23">
+        <f t="shared" si="5"/>
+        <v>0.4</v>
+      </c>
+      <c r="I28" s="23">
+        <f t="shared" si="6"/>
+        <v>0.24</v>
+      </c>
+      <c r="J28" s="23">
+        <f t="shared" si="7"/>
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B29" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="C29" s="36">
+        <v>10</v>
+      </c>
+      <c r="D29" s="14">
+        <v>10</v>
+      </c>
+      <c r="E29" s="13">
+        <v>5</v>
+      </c>
+      <c r="F29" s="13">
+        <v>2</v>
+      </c>
+      <c r="G29" s="22">
+        <f t="shared" si="4"/>
+        <v>0.4</v>
+      </c>
+      <c r="H29" s="23">
+        <f t="shared" si="5"/>
+        <v>0.4</v>
+      </c>
+      <c r="I29" s="23">
+        <f t="shared" si="6"/>
+        <v>0.2</v>
+      </c>
+      <c r="J29" s="23">
+        <f t="shared" si="7"/>
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B30" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="C30" s="36">
+        <v>18</v>
+      </c>
+      <c r="D30" s="14">
+        <v>10</v>
+      </c>
+      <c r="E30" s="13">
+        <v>6</v>
+      </c>
+      <c r="F30" s="13">
+        <v>2</v>
+      </c>
+      <c r="G30" s="22">
+        <f t="shared" si="4"/>
+        <v>0.72</v>
+      </c>
+      <c r="H30" s="23">
+        <f t="shared" si="5"/>
+        <v>0.4</v>
+      </c>
+      <c r="I30" s="23">
+        <f t="shared" si="6"/>
+        <v>0.24</v>
+      </c>
+      <c r="J30" s="23">
+        <f t="shared" si="7"/>
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B31" s="30">
+        <v>4</v>
+      </c>
+      <c r="C31" s="36">
+        <v>0</v>
+      </c>
+      <c r="D31" s="14">
+        <v>12</v>
+      </c>
+      <c r="E31" s="13">
+        <v>25</v>
+      </c>
+      <c r="F31" s="13">
+        <v>3</v>
+      </c>
+      <c r="G31" s="22">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H31" s="23">
+        <f t="shared" si="5"/>
+        <v>0.48</v>
+      </c>
+      <c r="I31" s="23">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="J31" s="23">
+        <f t="shared" si="7"/>
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B32" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="C32" s="40">
+        <v>7</v>
+      </c>
+      <c r="D32" s="41">
+        <v>3</v>
+      </c>
+      <c r="E32" s="41">
+        <v>4</v>
+      </c>
+      <c r="F32" s="41">
+        <v>4</v>
+      </c>
+      <c r="G32" s="22">
+        <f t="shared" si="4"/>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="H32" s="23">
+        <f t="shared" si="5"/>
+        <v>0.12</v>
+      </c>
+      <c r="I32" s="23">
+        <f t="shared" si="6"/>
+        <v>0.16</v>
+      </c>
+      <c r="J32" s="23">
+        <f t="shared" si="7"/>
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B33" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="C33" s="40">
+        <v>15</v>
+      </c>
+      <c r="D33" s="41">
+        <v>3</v>
+      </c>
+      <c r="E33" s="41">
+        <v>4</v>
+      </c>
+      <c r="F33" s="41">
+        <v>4</v>
+      </c>
+      <c r="G33" s="22">
+        <f t="shared" si="4"/>
+        <v>0.6</v>
+      </c>
+      <c r="H33" s="23">
+        <f t="shared" si="5"/>
+        <v>0.12</v>
+      </c>
+      <c r="I33" s="23">
+        <f t="shared" si="6"/>
+        <v>0.16</v>
+      </c>
+      <c r="J33" s="23">
+        <f t="shared" si="7"/>
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B34" s="39">
+        <v>6</v>
+      </c>
+      <c r="C34" s="40">
+        <v>11</v>
+      </c>
+      <c r="D34" s="41">
+        <v>7</v>
+      </c>
+      <c r="E34" s="41">
+        <v>3</v>
+      </c>
+      <c r="F34" s="41">
+        <v>3</v>
+      </c>
+      <c r="G34" s="22">
+        <f t="shared" si="4"/>
+        <v>0.44</v>
+      </c>
+      <c r="H34" s="23">
+        <f t="shared" si="5"/>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="I34" s="23">
+        <f t="shared" si="6"/>
+        <v>0.12</v>
+      </c>
+      <c r="J34" s="23">
+        <f t="shared" si="7"/>
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B35" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="C35" s="36">
+        <v>4</v>
+      </c>
+      <c r="D35" s="14">
+        <v>15</v>
+      </c>
+      <c r="E35" s="13">
+        <v>4</v>
+      </c>
+      <c r="F35" s="13">
+        <v>3</v>
+      </c>
+      <c r="G35" s="22">
+        <f t="shared" si="4"/>
+        <v>0.16</v>
+      </c>
+      <c r="H35" s="23">
+        <f t="shared" si="5"/>
+        <v>0.6</v>
+      </c>
+      <c r="I35" s="23">
+        <f t="shared" si="6"/>
+        <v>0.16</v>
+      </c>
+      <c r="J35" s="23">
+        <f t="shared" si="7"/>
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B36" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="C36" s="36">
+        <v>14</v>
+      </c>
+      <c r="D36" s="14">
+        <v>15</v>
+      </c>
+      <c r="E36" s="13">
+        <v>4</v>
+      </c>
+      <c r="F36" s="13">
+        <v>3</v>
+      </c>
+      <c r="G36" s="22">
+        <f t="shared" si="4"/>
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="H36" s="23">
+        <f t="shared" si="5"/>
+        <v>0.6</v>
+      </c>
+      <c r="I36" s="23">
+        <f t="shared" si="6"/>
+        <v>0.16</v>
+      </c>
+      <c r="J36" s="23">
+        <f t="shared" si="7"/>
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B37" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="C37" s="36">
+        <v>3</v>
+      </c>
+      <c r="D37" s="14">
+        <v>18</v>
+      </c>
+      <c r="E37" s="13">
+        <v>2</v>
+      </c>
+      <c r="F37" s="13">
+        <v>3</v>
+      </c>
+      <c r="G37" s="22">
+        <f t="shared" si="4"/>
+        <v>0.12</v>
+      </c>
+      <c r="H37" s="23">
+        <f t="shared" si="5"/>
+        <v>0.72</v>
+      </c>
+      <c r="I37" s="23">
+        <f t="shared" si="6"/>
+        <v>0.08</v>
+      </c>
+      <c r="J37" s="23">
+        <f t="shared" si="7"/>
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B38" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="C38" s="36">
+        <v>9</v>
+      </c>
+      <c r="D38" s="14">
+        <v>18</v>
+      </c>
+      <c r="E38" s="13">
+        <v>5</v>
+      </c>
+      <c r="F38" s="13">
+        <v>3</v>
+      </c>
+      <c r="G38" s="22">
+        <f t="shared" si="4"/>
+        <v>0.36</v>
+      </c>
+      <c r="H38" s="23">
+        <f t="shared" si="5"/>
+        <v>0.72</v>
+      </c>
+      <c r="I38" s="23">
+        <f t="shared" si="6"/>
+        <v>0.2</v>
+      </c>
+      <c r="J38" s="23">
+        <f t="shared" si="7"/>
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B39" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="C39" s="36">
+        <v>18</v>
+      </c>
+      <c r="D39" s="14">
+        <v>18</v>
+      </c>
+      <c r="E39" s="13">
+        <v>2</v>
+      </c>
+      <c r="F39" s="13">
+        <v>3</v>
+      </c>
+      <c r="G39" s="22">
+        <f t="shared" si="4"/>
+        <v>0.72</v>
+      </c>
+      <c r="H39" s="23">
+        <f t="shared" si="5"/>
+        <v>0.72</v>
+      </c>
+      <c r="I39" s="23">
+        <f t="shared" si="6"/>
+        <v>0.08</v>
+      </c>
+      <c r="J39" s="23">
+        <f t="shared" si="7"/>
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B40" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="C40" s="36">
+        <v>0</v>
+      </c>
+      <c r="D40" s="14">
+        <v>21</v>
+      </c>
+      <c r="E40" s="13">
+        <v>4</v>
+      </c>
+      <c r="F40" s="13">
+        <v>4</v>
+      </c>
+      <c r="G40" s="22">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H40" s="23">
+        <f t="shared" si="5"/>
+        <v>0.84</v>
+      </c>
+      <c r="I40" s="23">
+        <f t="shared" si="6"/>
+        <v>0.16</v>
+      </c>
+      <c r="J40" s="23">
+        <f t="shared" si="7"/>
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B41" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="C41" s="36">
+        <v>5</v>
+      </c>
+      <c r="D41" s="14">
+        <v>21</v>
+      </c>
+      <c r="E41" s="13">
+        <v>4</v>
+      </c>
+      <c r="F41" s="13">
+        <v>4</v>
+      </c>
+      <c r="G41" s="22">
+        <f t="shared" si="4"/>
+        <v>0.2</v>
+      </c>
+      <c r="H41" s="23">
+        <f t="shared" si="5"/>
+        <v>0.84</v>
+      </c>
+      <c r="I41" s="23">
+        <f t="shared" si="6"/>
+        <v>0.16</v>
+      </c>
+      <c r="J41" s="23">
+        <f t="shared" si="7"/>
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B42" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="C42" s="36">
+        <v>14</v>
+      </c>
+      <c r="D42" s="14">
+        <v>21</v>
+      </c>
+      <c r="E42" s="13">
+        <v>4</v>
+      </c>
+      <c r="F42" s="13">
+        <v>4</v>
+      </c>
+      <c r="G42" s="22">
+        <f t="shared" si="4"/>
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="H42" s="23">
+        <f t="shared" si="5"/>
+        <v>0.84</v>
+      </c>
+      <c r="I42" s="23">
+        <f t="shared" si="6"/>
+        <v>0.16</v>
+      </c>
+      <c r="J42" s="23">
+        <f t="shared" si="7"/>
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B43" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="C43" s="36">
+        <v>20</v>
+      </c>
+      <c r="D43" s="14">
+        <v>21</v>
+      </c>
+      <c r="E43" s="13">
+        <v>4</v>
+      </c>
+      <c r="F43" s="13">
+        <v>4</v>
+      </c>
+      <c r="G43" s="22">
+        <f t="shared" si="4"/>
+        <v>0.8</v>
+      </c>
+      <c r="H43" s="23">
+        <f t="shared" si="5"/>
+        <v>0.84</v>
+      </c>
+      <c r="I43" s="23">
+        <f t="shared" si="6"/>
+        <v>0.16</v>
+      </c>
+      <c r="J43" s="23">
+        <f t="shared" si="7"/>
+        <v>0.16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <tableParts count="2">
-    <tablePart r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="4">
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ajustado o sprite do Lulanos e adicionado pontos
</commit_message>
<xml_diff>
--- a/assets/dados.xlsx
+++ b/assets/dados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\Treinamentos\Python\meu-jogo\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5600AE23-74B3-4A48-A180-3858703DAA13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5CE725E-65E6-4543-9891-EC8747BA7A6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-165" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{D0AC3F4F-C2BF-45A5-B453-A20E0A07E23C}"/>
   </bookViews>
@@ -6026,7 +6026,7 @@
   <dimension ref="B1:J43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A18" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+      <selection activeCell="G36" sqref="G36:J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6917,7 +6917,7 @@
         <v>72</v>
       </c>
       <c r="C33" s="40">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D33" s="41">
         <v>3</v>
@@ -6930,7 +6930,7 @@
       </c>
       <c r="G33" s="22">
         <f t="shared" si="4"/>
-        <v>0.6</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="H33" s="23">
         <f t="shared" si="5"/>
@@ -6983,7 +6983,7 @@
         <v>76</v>
       </c>
       <c r="C35" s="36">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D35" s="14">
         <v>15</v>
@@ -6996,7 +6996,7 @@
       </c>
       <c r="G35" s="22">
         <f t="shared" si="4"/>
-        <v>0.16</v>
+        <v>0.24</v>
       </c>
       <c r="H35" s="23">
         <f t="shared" si="5"/>
@@ -7016,7 +7016,7 @@
         <v>77</v>
       </c>
       <c r="C36" s="36">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D36" s="14">
         <v>15</v>
@@ -7029,7 +7029,7 @@
       </c>
       <c r="G36" s="22">
         <f t="shared" si="4"/>
-        <v>0.56000000000000005</v>
+        <v>0.6</v>
       </c>
       <c r="H36" s="23">
         <f t="shared" si="5"/>

</xml_diff>